<commit_message>
Cost Modeling First Attempt
Developed basic cost modeling test case in the ISP reviews workbook,
experience some order of magnitude problems to be worked out
</commit_message>
<xml_diff>
--- a/MSDO/Assignment2/ISP reviews.xlsx
+++ b/MSDO/Assignment2/ISP reviews.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Isp</t>
   </si>
@@ -34,14 +34,153 @@
   </si>
   <si>
     <t>Electric Propulsion</t>
+  </si>
+  <si>
+    <t>NASA Advanced Mission Cost Model (from HSMAD)</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>zi</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>dry mass (lbs)</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>specification</t>
+  </si>
+  <si>
+    <t>IOC</t>
+  </si>
+  <si>
+    <t>initial operating capability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B </t>
+  </si>
+  <si>
+    <t>Block number</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>1999-2016 Inflation</t>
+  </si>
+  <si>
+    <t>http://ntrs.nasa.gov/archive/nasa/casi.ntrs.nasa.gov/20140005340.pdf</t>
+  </si>
+  <si>
+    <t>http://ntrs.nasa.gov/archive/nasa/casi.ntrs.nasa.gov/20140005476.pdf</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/sites/default/files/files/CEH_AppD.pdf</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/sites/default/files/files/01_CEH_Main_Body_02_27_15.pdf</t>
+  </si>
+  <si>
+    <t>Inertr Mass Ratio</t>
+  </si>
+  <si>
+    <t>What about the electric propulsion nuclear generator or solar panel mass?  NTR reactor mass seems high?</t>
+  </si>
+  <si>
+    <t>Total Development Cost ($M 1999)</t>
+  </si>
+  <si>
+    <t>Total Development Cost ($M 2016)</t>
+  </si>
+  <si>
+    <t>Prop Mass (kg)</t>
+  </si>
+  <si>
+    <t>Engine Mass (kg)</t>
+  </si>
+  <si>
+    <t>Static Engine Mass (kg)</t>
+  </si>
+  <si>
+    <t>SSME weights 7,775</t>
+  </si>
+  <si>
+    <t>These prices are WAY too high… the mass seems to be really large for these based on what I'd expect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,13 +205,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -192,11 +349,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91446272"/>
-        <c:axId val="91444736"/>
+        <c:axId val="41240448"/>
+        <c:axId val="41692160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91446272"/>
+        <c:axId val="41240448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="485"/>
@@ -226,12 +383,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91444736"/>
+        <c:crossAx val="41692160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91444736"/>
+        <c:axId val="41692160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -261,7 +418,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91446272"/>
+        <c:crossAx val="41240448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -386,11 +543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95582848"/>
-        <c:axId val="95732864"/>
+        <c:axId val="47000192"/>
+        <c:axId val="50230016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95582848"/>
+        <c:axId val="47000192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="485"/>
@@ -420,12 +577,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95732864"/>
+        <c:crossAx val="50230016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95732864"/>
+        <c:axId val="50230016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +611,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95582848"/>
+        <c:crossAx val="47000192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -572,11 +729,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95731712"/>
-        <c:axId val="95716864"/>
+        <c:axId val="46973312"/>
+        <c:axId val="46975232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95731712"/>
+        <c:axId val="46973312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,12 +762,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95716864"/>
+        <c:crossAx val="46975232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95716864"/>
+        <c:axId val="46975232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -640,7 +797,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95731712"/>
+        <c:crossAx val="46973312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -765,11 +922,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104902016"/>
-        <c:axId val="105092608"/>
+        <c:axId val="47040768"/>
+        <c:axId val="47042944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104902016"/>
+        <c:axId val="47040768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2500"/>
@@ -799,12 +956,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105092608"/>
+        <c:crossAx val="47042944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105092608"/>
+        <c:axId val="47042944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -834,7 +991,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104902016"/>
+        <c:crossAx val="47040768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -1270,15 +1427,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:T10"/>
+  <dimension ref="A5:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6:T10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
@@ -1428,9 +1588,589 @@
         <v>4</v>
       </c>
     </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1">
+        <v>5.6499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>0.59409999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>0.66039999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>80.599000000000004</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="3">
+        <v>3.8084999999999997E-55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>-0.3553</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>1.5690999999999999</v>
+      </c>
+      <c r="E57" s="6">
+        <v>445</v>
+      </c>
+      <c r="F57" s="6">
+        <v>452</v>
+      </c>
+      <c r="G57" s="6">
+        <v>465</v>
+      </c>
+      <c r="H57" s="6">
+        <v>480</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7">
+        <v>850</v>
+      </c>
+      <c r="K57" s="7">
+        <v>950</v>
+      </c>
+      <c r="L57" s="7">
+        <v>1000</v>
+      </c>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7">
+        <v>3000</v>
+      </c>
+      <c r="O57" s="7">
+        <v>3800</v>
+      </c>
+      <c r="P57" s="7">
+        <v>5000</v>
+      </c>
+      <c r="Q57" s="7">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="9">
+        <f>F59*0.95</f>
+        <v>44433.4</v>
+      </c>
+      <c r="F59" s="9">
+        <f>F69*2.2/F58</f>
+        <v>46772.000000000007</v>
+      </c>
+      <c r="G59" s="9">
+        <f>F59*1.1</f>
+        <v>51449.200000000012</v>
+      </c>
+      <c r="H59" s="9">
+        <f>F59*1.25</f>
+        <v>58465.000000000007</v>
+      </c>
+      <c r="J59" s="9">
+        <f>J69*2.2</f>
+        <v>96326.34</v>
+      </c>
+      <c r="K59" s="9">
+        <f>J59*1.1</f>
+        <v>105958.974</v>
+      </c>
+      <c r="L59" s="9">
+        <f>J59*1.15</f>
+        <v>110775.29099999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60">
+        <v>2.39</v>
+      </c>
+      <c r="F60">
+        <v>2.39</v>
+      </c>
+      <c r="G60">
+        <v>2.39</v>
+      </c>
+      <c r="H60">
+        <v>2.39</v>
+      </c>
+      <c r="J60">
+        <v>2.39</v>
+      </c>
+      <c r="K60">
+        <v>2.39</v>
+      </c>
+      <c r="L60">
+        <v>2.39</v>
+      </c>
+      <c r="N60">
+        <v>2.39</v>
+      </c>
+      <c r="O60">
+        <v>2.39</v>
+      </c>
+      <c r="P60">
+        <v>2.39</v>
+      </c>
+      <c r="Q60">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61">
+        <v>2030</v>
+      </c>
+      <c r="F61">
+        <v>2030</v>
+      </c>
+      <c r="G61">
+        <v>2030</v>
+      </c>
+      <c r="H61">
+        <v>2030</v>
+      </c>
+      <c r="J61">
+        <v>2030</v>
+      </c>
+      <c r="K61">
+        <v>2030</v>
+      </c>
+      <c r="L61">
+        <v>2030</v>
+      </c>
+      <c r="N61">
+        <v>2030</v>
+      </c>
+      <c r="O61">
+        <v>2030</v>
+      </c>
+      <c r="P61">
+        <v>2030</v>
+      </c>
+      <c r="Q61">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63">
+        <v>-1.5</v>
+      </c>
+      <c r="F63">
+        <v>-0.5</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1.5</v>
+      </c>
+      <c r="K63">
+        <v>1.5</v>
+      </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
+      <c r="N63">
+        <v>0.5</v>
+      </c>
+      <c r="O63">
+        <v>0.5</v>
+      </c>
+      <c r="P63">
+        <v>1</v>
+      </c>
+      <c r="Q63">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="J66" s="8">
+        <v>34500</v>
+      </c>
+      <c r="K66">
+        <f>J66*1.05</f>
+        <v>36225</v>
+      </c>
+      <c r="L66">
+        <f>J66*1.1</f>
+        <v>37950</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67">
+        <v>0.17</v>
+      </c>
+      <c r="F67">
+        <v>0.18</v>
+      </c>
+      <c r="G67">
+        <v>0.19</v>
+      </c>
+      <c r="H67">
+        <v>0.2</v>
+      </c>
+      <c r="J67">
+        <v>0.1</v>
+      </c>
+      <c r="K67">
+        <v>0.11</v>
+      </c>
+      <c r="L67">
+        <v>0.12</v>
+      </c>
+      <c r="N67">
+        <v>0.18</v>
+      </c>
+      <c r="O67">
+        <v>0.19</v>
+      </c>
+      <c r="P67">
+        <v>0.2</v>
+      </c>
+      <c r="Q67">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68">
+        <v>125060</v>
+      </c>
+      <c r="J68">
+        <v>92847</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F69">
+        <v>21260</v>
+      </c>
+      <c r="J69" s="9">
+        <f>J66+J68*0.1</f>
+        <v>43784.7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>SUM(F68:F69)</f>
+        <v>146320</v>
+      </c>
+      <c r="J70">
+        <f>SUM(J68:J69)</f>
+        <v>136631.70000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" s="10">
+        <f>$B$51*E58^$B$52*E59*$B$53*$B$54^E60*$B$55^(1/(E61-1900))*E62^$B$56*$B$57^E63</f>
+        <v>78358.521011129968</v>
+      </c>
+      <c r="F73" s="10">
+        <f>$B$51*F58^$B$52*F59*$B$53*$B$54^F60*$B$55^(1/(F61-1900))*F62^$B$56*$B$57^F63</f>
+        <v>129423.53191427796</v>
+      </c>
+      <c r="G73" s="10">
+        <f t="shared" ref="G73:H73" si="0">$B$51*G58^$B$52*G59*$B$53*$B$54^G60*$B$55^(1/(G61-1900))*G62^$B$56*$B$57^G63</f>
+        <v>205966.4426147528</v>
+      </c>
+      <c r="H73" s="10">
+        <f t="shared" si="0"/>
+        <v>469807.96539144288</v>
+      </c>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10">
+        <f t="shared" ref="I73:L73" si="1">$B$51*J58^$B$52*J59*$B$53*$B$54^J60*$B$55^(1/(J61-1900))*J62^$B$56*$B$57^J63</f>
+        <v>969604.87901508925</v>
+      </c>
+      <c r="K73" s="10">
+        <f t="shared" si="1"/>
+        <v>1066565.3669165981</v>
+      </c>
+      <c r="L73" s="10">
+        <f t="shared" si="1"/>
+        <v>1396747.6319761402</v>
+      </c>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+      <c r="O73" s="10"/>
+      <c r="P73" s="10"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="10">
+        <f>E73*$G$54</f>
+        <v>111269.09983580455</v>
+      </c>
+      <c r="F74" s="10">
+        <f t="shared" ref="F74:H74" si="2">F73*$G$54</f>
+        <v>183781.4153182747</v>
+      </c>
+      <c r="G74" s="10">
+        <f t="shared" si="2"/>
+        <v>292472.34851294896</v>
+      </c>
+      <c r="H74" s="10">
+        <f t="shared" si="2"/>
+        <v>667127.31085584883</v>
+      </c>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10">
+        <f t="shared" ref="J74" si="3">J73*$G$54</f>
+        <v>1376838.9282014268</v>
+      </c>
+      <c r="K74" s="10">
+        <f t="shared" ref="K74" si="4">K73*$G$54</f>
+        <v>1514522.8210215692</v>
+      </c>
+      <c r="L74" s="10">
+        <f t="shared" ref="L74" si="5">L73*$G$54</f>
+        <v>1983381.6374061189</v>
+      </c>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E56:H56"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="N56:Q56"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E54" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated ISP AMCM values
new AMCM values
</commit_message>
<xml_diff>
--- a/MSDO/Assignment2/ISP reviews.xlsx
+++ b/MSDO/Assignment2/ISP reviews.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cces\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Isp</t>
   </si>
@@ -140,7 +135,13 @@
     <t>SSME weights 7,775</t>
   </si>
   <si>
-    <t>These prices are WAY too high… the mass seems to be really large for these based on what I'd expect</t>
+    <t>http://www.esa.int/Our_Activities/Human_Spaceflight/Space_Shuttle/Shuttle_technical_facts</t>
+  </si>
+  <si>
+    <t>The NTR does not seem to be reasonable as it doesn’t reduce propellant mass by all that much….</t>
+  </si>
+  <si>
+    <t>Total engine and propulsion mas (kg)</t>
   </si>
 </sst>
 </file>
@@ -356,11 +357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169146240"/>
-        <c:axId val="168322352"/>
+        <c:axId val="47951872"/>
+        <c:axId val="47954176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169146240"/>
+        <c:axId val="47951872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="485"/>
@@ -389,12 +390,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168322352"/>
+        <c:crossAx val="47954176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168322352"/>
+        <c:axId val="47954176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -423,7 +424,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169146240"/>
+        <c:crossAx val="47951872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -548,11 +549,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167375680"/>
-        <c:axId val="167376464"/>
+        <c:axId val="55450624"/>
+        <c:axId val="78626176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167375680"/>
+        <c:axId val="55450624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="485"/>
@@ -582,12 +583,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167376464"/>
+        <c:crossAx val="78626176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167376464"/>
+        <c:axId val="78626176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +617,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167375680"/>
+        <c:crossAx val="55450624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -733,11 +734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167377248"/>
-        <c:axId val="125196528"/>
+        <c:axId val="51437952"/>
+        <c:axId val="51439872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167377248"/>
+        <c:axId val="51437952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,12 +766,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125196528"/>
+        <c:crossAx val="51439872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125196528"/>
+        <c:axId val="51439872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -799,7 +800,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167377248"/>
+        <c:crossAx val="51437952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -923,11 +924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125198488"/>
-        <c:axId val="125191040"/>
+        <c:axId val="54692096"/>
+        <c:axId val="58392960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125198488"/>
+        <c:axId val="54692096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2500"/>
@@ -956,12 +957,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125191040"/>
+        <c:crossAx val="58392960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125191040"/>
+        <c:axId val="58392960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -990,7 +991,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125198488"/>
+        <c:crossAx val="54692096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -1182,7 +1183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1217,7 +1218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1426,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:T82"/>
+  <dimension ref="A5:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,10 +1864,10 @@
         <v>23</v>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G62">
         <v>2</v>
@@ -1904,19 +1905,19 @@
         <v>25</v>
       </c>
       <c r="E63">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="F63">
         <v>-2</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H63">
         <v>1</v>
       </c>
       <c r="J63">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -2040,8 +2041,14 @@
         <f>J66+J68*0.1</f>
         <v>43784.7</v>
       </c>
+      <c r="R69" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
       <c r="F70">
         <f>SUM(F68:F69)</f>
         <v>146320</v>
@@ -2057,15 +2064,15 @@
       </c>
       <c r="E73" s="9">
         <f t="shared" ref="E73:G73" si="0">$B$51*E58^$B$52*E59^$B$53*$B$54^E60*$B$55^(1/(E61-1900))*E62^$B$56*$B$57^E63</f>
-        <v>2500.8733149891486</v>
+        <v>1560.6676341627724</v>
       </c>
       <c r="F73" s="9">
         <f t="shared" si="0"/>
-        <v>2587.0392846159261</v>
+        <v>2022.3069115960209</v>
       </c>
       <c r="G73" s="9">
         <f t="shared" si="0"/>
-        <v>7834.390629108686</v>
+        <v>4992.9199089342219</v>
       </c>
       <c r="H73" s="9">
         <f>$B$51*H58^$B$52*H59^$B$53*$B$54^H60*$B$55^(1/(H61-1900))*H62^$B$56*$B$57^H63</f>
@@ -2073,8 +2080,8 @@
       </c>
       <c r="I73" s="9"/>
       <c r="J73" s="9">
-        <f t="shared" ref="J73:M73" si="1">$B$51*J58^$B$52*J59^$B$53*$B$54^J60*$B$55^(1/(J61-1900))*J62^$B$56*$B$57^J63</f>
-        <v>23794.82933758236</v>
+        <f t="shared" ref="J73:L73" si="1">$B$51*J58^$B$52*J59^$B$53*$B$54^J60*$B$55^(1/(J61-1900))*J62^$B$56*$B$57^J63</f>
+        <v>18995.786645201308</v>
       </c>
       <c r="K73" s="9">
         <f t="shared" si="1"/>
@@ -2089,9 +2096,7 @@
       <c r="O73" s="9"/>
       <c r="P73" s="9"/>
       <c r="Q73" s="9"/>
-      <c r="R73" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="R73" s="9"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -2099,15 +2104,15 @@
       </c>
       <c r="E74" s="9">
         <f>E73*$G$54</f>
-        <v>3551.240107284591</v>
+        <v>2216.1480405111365</v>
       </c>
       <c r="F74" s="9">
         <f t="shared" ref="F74:H74" si="2">F73*$G$54</f>
-        <v>3673.5957841546151</v>
+        <v>2871.6758144663495</v>
       </c>
       <c r="G74" s="9">
         <f t="shared" si="2"/>
-        <v>11124.834693334333</v>
+        <v>7089.9462706865943</v>
       </c>
       <c r="H74" s="9">
         <f t="shared" si="2"/>
@@ -2116,7 +2121,7 @@
       <c r="I74" s="9"/>
       <c r="J74" s="9">
         <f t="shared" ref="J74" si="3">J73*$G$54</f>
-        <v>33788.657659366952</v>
+        <v>26974.017036185855</v>
       </c>
       <c r="K74" s="9">
         <f t="shared" ref="K74" si="4">K73*$G$54</f>
@@ -2156,6 +2161,11 @@
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Isp Development Cost Module
Adds a new module to calculate development cost for transit engines
based on type and Isp. Updates results class to add in development
costs. This module must be UPDATED once new Isp ranges are put into the
code, currently works for the old Isp values.
</commit_message>
<xml_diff>
--- a/MSDO/Assignment2/ISP reviews.xlsx
+++ b/MSDO/Assignment2/ISP reviews.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>Isp</t>
   </si>
@@ -142,6 +142,54 @@
   </si>
   <si>
     <t>Total engine and propulsion mas (kg)</t>
+  </si>
+  <si>
+    <t>http://www.thespacereview.com/article/1579/1</t>
+  </si>
+  <si>
+    <t>Program Commenced</t>
+  </si>
+  <si>
+    <t>Program Retired</t>
+  </si>
+  <si>
+    <t>First Enterprise in Air Flight Test</t>
+  </si>
+  <si>
+    <t>First Space-Worthy shuttle launch - Columia STS 1</t>
+  </si>
+  <si>
+    <t>Columbia manufactured and delivered</t>
+  </si>
+  <si>
+    <t>Challenger delivered</t>
+  </si>
+  <si>
+    <t>Discovery</t>
+  </si>
+  <si>
+    <t>Atlantis</t>
+  </si>
+  <si>
+    <t>NASA Original Price Estimate</t>
+  </si>
+  <si>
+    <t>2011 $</t>
+  </si>
+  <si>
+    <t>% of total</t>
+  </si>
+  <si>
+    <t>NRE</t>
+  </si>
+  <si>
+    <t>Challenger Disaster</t>
+  </si>
+  <si>
+    <t>Columbia Disaster</t>
+  </si>
+  <si>
+    <t>Endeavour built to replace Challenger</t>
   </si>
 </sst>
 </file>
@@ -281,6 +329,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -357,11 +406,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47951872"/>
-        <c:axId val="47954176"/>
+        <c:axId val="105672704"/>
+        <c:axId val="105674624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47951872"/>
+        <c:axId val="105672704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="485"/>
@@ -384,18 +433,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47954176"/>
+        <c:crossAx val="105674624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47954176"/>
+        <c:axId val="105674624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -418,13 +468,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47951872"/>
+        <c:crossAx val="105672704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -549,11 +600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55450624"/>
-        <c:axId val="78626176"/>
+        <c:axId val="105691008"/>
+        <c:axId val="105705472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55450624"/>
+        <c:axId val="105691008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="485"/>
@@ -583,12 +634,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78626176"/>
+        <c:crossAx val="105705472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78626176"/>
+        <c:axId val="105705472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +668,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55450624"/>
+        <c:crossAx val="105691008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -664,6 +715,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -734,11 +786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51437952"/>
-        <c:axId val="51439872"/>
+        <c:axId val="105066496"/>
+        <c:axId val="105068416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51437952"/>
+        <c:axId val="105066496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,18 +812,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51439872"/>
+        <c:crossAx val="105068416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51439872"/>
+        <c:axId val="105068416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -794,13 +847,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51437952"/>
+        <c:crossAx val="105066496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -848,6 +902,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -924,11 +979,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54692096"/>
-        <c:axId val="58392960"/>
+        <c:axId val="131598208"/>
+        <c:axId val="131600384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54692096"/>
+        <c:axId val="131598208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2500"/>
@@ -951,18 +1006,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58392960"/>
+        <c:crossAx val="131600384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58392960"/>
+        <c:axId val="131600384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -985,18 +1041,188 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54692096"/>
+        <c:crossAx val="131598208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$78:$I$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$78:$J$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>26974.017036185855</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40718.104055823904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51808.779917026295</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61465.223947798768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70178.439515539343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78206.938508149193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85707.410338511967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92783.63623643943</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99508.711397715044</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>105936.50173927273</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>134791.1704401827</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="47012096"/>
+        <c:axId val="47010560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="47012096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47010560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="47010560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47012096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1135,6 +1361,91 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>446995</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>52917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="chart"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="18510250"/>
+          <a:ext cx="6151412" cy="3640667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1427,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:T85"/>
+  <dimension ref="A5:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,29 +2454,233 @@
         <v>38</v>
       </c>
     </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>26974.017036185855</v>
+      </c>
+    </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>30</v>
       </c>
+      <c r="I79">
+        <v>2</v>
+      </c>
+      <c r="J79">
+        <v>40718.104055823904</v>
+      </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>3</v>
+      </c>
+      <c r="J80">
+        <v>51808.779917026295</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>4</v>
+      </c>
+      <c r="J81">
+        <v>61465.223947798768</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>5</v>
+      </c>
+      <c r="J82">
+        <v>70178.439515539343</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>6</v>
+      </c>
+      <c r="J83">
+        <v>78206.938508149193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>7</v>
+      </c>
+      <c r="J84">
+        <v>85707.410338511967</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>39</v>
+      </c>
+      <c r="I85">
+        <v>8</v>
+      </c>
+      <c r="J85">
+        <v>92783.63623643943</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>9</v>
+      </c>
+      <c r="J86">
+        <v>99508.711397715044</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <v>10</v>
+      </c>
+      <c r="J87">
+        <v>105936.50173927273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>15</v>
+      </c>
+      <c r="J88">
+        <v>134791.1704401827</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <v>20</v>
+      </c>
+      <c r="J89">
+        <v>159914.39077624356</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <v>50</v>
+      </c>
+      <c r="J90">
+        <v>275615.54401867534</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q98" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J99">
+        <v>1972</v>
+      </c>
+      <c r="K99" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>52</v>
+      </c>
+      <c r="R99" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J100">
+        <v>1977</v>
+      </c>
+      <c r="K100" t="s">
+        <v>45</v>
+      </c>
+      <c r="P100" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q100" s="7">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J101">
+        <v>1979</v>
+      </c>
+      <c r="K101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J102">
+        <v>1981</v>
+      </c>
+      <c r="K102" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J103">
+        <v>1982</v>
+      </c>
+      <c r="K103" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J104">
+        <v>1983</v>
+      </c>
+      <c r="K104" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J105">
+        <v>1985</v>
+      </c>
+      <c r="K105" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J106">
+        <v>1986</v>
+      </c>
+      <c r="K106" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J107">
+        <v>1991</v>
+      </c>
+      <c r="K107" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J108">
+        <v>2003</v>
+      </c>
+      <c r="K108" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J109">
+        <v>2011</v>
+      </c>
+      <c r="K109" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>